<commit_message>
añadir vista indexar y mostrar empleados, pendiente de verificacion. intento de añadir informacion a la base de datos. crear html empleados_detail y empleados_index, no rellenar por dentro
</commit_message>
<xml_diff>
--- a/Gant - Ingeniería WEB.xlsx
+++ b/Gant - Ingeniería WEB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deusto\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deusto\Desktop\Nueva carpeta\2ºCURSO\2º CUATRIMESTRE\INGENIERÍA WEB\PROYECTO IW\deustoGes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D62904-D6EF-4E22-8547-0FB27596FE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5441A5A-EB44-4D3E-9B9B-C6762ABCD8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E42BD46-7C25-4210-B3F0-CB7F1A8D30BC}"/>
   </bookViews>
@@ -230,6 +230,62 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Conector recto 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49E201FD-CB40-7DEF-14B8-2840CE922ADE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5734050" y="762000"/>
+          <a:ext cx="0" cy="2619375"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -552,7 +608,7 @@
   <dimension ref="B2:U27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,11 +705,11 @@
       <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
+      <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>12</v>
@@ -825,5 +881,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
añadir funciones en view, crear urls, actualizar gant
</commit_message>
<xml_diff>
--- a/Gant - Ingeniería WEB.xlsx
+++ b/Gant - Ingeniería WEB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deusto\Desktop\Nueva carpeta\2ºCURSO\2º CUATRIMESTRE\INGENIERÍA WEB\PROYECTO IW\deustoGes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5441A5A-EB44-4D3E-9B9B-C6762ABCD8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDE8D1D-D13B-4FB0-A044-ED3CED15B617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E42BD46-7C25-4210-B3F0-CB7F1A8D30BC}"/>
   </bookViews>
@@ -198,7 +198,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -206,6 +206,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -236,14 +237,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
@@ -260,7 +261,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5734050" y="762000"/>
+          <a:off x="6534150" y="762000"/>
           <a:ext cx="0" cy="2619375"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -608,7 +609,7 @@
   <dimension ref="B2:U27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,7 +712,7 @@
       <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -727,16 +728,16 @@
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>10</v>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>10</v>
+      <c r="F10" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>10</v>
@@ -767,8 +768,8 @@
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>10</v>
+      <c r="F11" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>10</v>
@@ -799,8 +800,8 @@
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>10</v>
+      <c r="F12" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
arreglar lo de los url, intentar hacer migraciones y meter datos sin éxito, añadir un __str__(self) que faltaba y pequeños cambios
</commit_message>
<xml_diff>
--- a/Gant - Ingeniería WEB.xlsx
+++ b/Gant - Ingeniería WEB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deusto\Desktop\Nueva carpeta\2ºCURSO\2º CUATRIMESTRE\INGENIERÍA WEB\PROYECTO IW\deustoGes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDE8D1D-D13B-4FB0-A044-ED3CED15B617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3693C8C4-A5C4-49A0-99E3-3FF17D208ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E42BD46-7C25-4210-B3F0-CB7F1A8D30BC}"/>
   </bookViews>
@@ -237,16 +237,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -261,7 +261,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6534150" y="762000"/>
+          <a:off x="8820150" y="733425"/>
           <a:ext cx="0" cy="2619375"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -609,7 +609,7 @@
   <dimension ref="B2:U27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,14 +739,14 @@
       <c r="F10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>10</v>
+      <c r="G10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>10</v>
@@ -771,14 +771,14 @@
       <c r="F11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>10</v>
+      <c r="G11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>10</v>
@@ -803,14 +803,14 @@
       <c r="F12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>10</v>
+      <c r="G12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
word de organizacion pantallas
</commit_message>
<xml_diff>
--- a/Gant - Ingeniería WEB.xlsx
+++ b/Gant - Ingeniería WEB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deusto\Desktop\Nueva carpeta\2ºCURSO\2º CUATRIMESTRE\INGENIERÍA WEB\PROYECTO IW\deustoGes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3693C8C4-A5C4-49A0-99E3-3FF17D208ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FC57DC-58C7-4085-8121-A9F6A5BC8EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E42BD46-7C25-4210-B3F0-CB7F1A8D30BC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="15">
   <si>
     <t>Tareas</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Puesta en común</t>
-  </si>
-  <si>
-    <t>Cada uno que se encargue de una entidad de la entidad relación</t>
   </si>
   <si>
     <t>Repartir las entidades para programar</t>
@@ -237,16 +234,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -261,7 +258,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8820150" y="733425"/>
+          <a:off x="13601700" y="704850"/>
           <a:ext cx="0" cy="2619375"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -606,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55842CA0-FB16-4CFF-991C-9D97933A8D49}">
-  <dimension ref="B2:U27"/>
+  <dimension ref="B2:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +723,7 @@
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>9</v>
@@ -748,19 +745,19 @@
       <c r="I10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N10" s="6" t="s">
+      <c r="J10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -780,19 +777,19 @@
       <c r="I11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" s="6" t="s">
+      <c r="J11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -812,19 +809,19 @@
       <c r="I12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12" s="6" t="s">
+      <c r="J12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -832,11 +829,20 @@
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
@@ -869,15 +875,10 @@
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S16" s="6" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inicio de css en pantalla clientes
</commit_message>
<xml_diff>
--- a/Gant - Ingeniería WEB.xlsx
+++ b/Gant - Ingeniería WEB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deusto\Desktop\Nueva carpeta\2ºCURSO\2º CUATRIMESTRE\INGENIERÍA WEB\PROYECTO IW\deustoGes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FC57DC-58C7-4085-8121-A9F6A5BC8EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07901B99-3A31-4B54-9130-2A808207A44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E42BD46-7C25-4210-B3F0-CB7F1A8D30BC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="15">
   <si>
     <t>Tareas</t>
   </si>
@@ -234,16 +234,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -258,7 +258,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13601700" y="704850"/>
+          <a:off x="18059400" y="1019175"/>
           <a:ext cx="0" cy="2619375"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -606,7 +606,7 @@
   <dimension ref="B2:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,39 +835,45 @@
       <c r="L13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>10</v>
+      <c r="M13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="P14" s="6" t="s">
-        <v>12</v>
+      <c r="O14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>3</v>
       </c>
-      <c r="P15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>10</v>
+      <c r="P15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R15" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="S15" s="6" t="s">
         <v>12</v>

</xml_diff>